<commit_message>
DA 19 | Day 1
</commit_message>
<xml_diff>
--- a/Batch/18/Day_2.xlsx
+++ b/Batch/18/Day_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29204"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Work\Acciojob\Modules\statistics\Batch\18\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\statistics\Batch\18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34903DC7-3496-4FC9-A272-529E75557FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90976C04-7A01-4B99-A989-CEC9BE797AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recap" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Data Vs Info</t>
   </si>
@@ -511,11 +511,17 @@
   <si>
     <t>True Zero</t>
   </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -649,8 +655,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -666,9 +691,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -693,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -708,31 +730,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{22C5263A-9319-452B-9309-C82F7F35DDBC}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1062,9 +1067,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="10.46484375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -1078,350 +1086,345 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E896BF5-0477-446D-A751-4DF4B102E8E8}">
   <dimension ref="L2:V33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="12:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L3" s="2" t="s">
+    <row r="2" spans="12:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="4"/>
-      <c r="R3" s="11" t="s">
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="11"/>
+      <c r="R3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="13"/>
-    </row>
-    <row r="4" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L4" s="5"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="7"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="16"/>
-    </row>
-    <row r="5" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="7"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="16"/>
-    </row>
-    <row r="6" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L6" s="5"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="7"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="16"/>
-    </row>
-    <row r="7" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L7" s="5"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="7"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="16"/>
-    </row>
-    <row r="8" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L8" s="5"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="7"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="16"/>
-    </row>
-    <row r="9" spans="12:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L9" s="8"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="10"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="19"/>
-    </row>
-    <row r="10" spans="12:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L11" s="2" t="s">
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="19"/>
+    </row>
+    <row r="4" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L4" s="12"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="13"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="22"/>
+    </row>
+    <row r="5" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L5" s="12"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="13"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="22"/>
+    </row>
+    <row r="6" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L6" s="12"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="13"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="22"/>
+    </row>
+    <row r="7" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L7" s="12"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="13"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="22"/>
+    </row>
+    <row r="8" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L8" s="12"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="13"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="22"/>
+    </row>
+    <row r="9" spans="12:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="16"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="25"/>
+    </row>
+    <row r="10" spans="12:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L11" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="4"/>
-      <c r="R11" s="11" t="s">
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="11"/>
+      <c r="R11" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="13"/>
-    </row>
-    <row r="12" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L12" s="5"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="7"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="16"/>
-    </row>
-    <row r="13" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L13" s="5"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="7"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="16"/>
-    </row>
-    <row r="14" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L14" s="5"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="7"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="16"/>
-    </row>
-    <row r="15" spans="12:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L15" s="8"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="10"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="19"/>
-    </row>
-    <row r="16" spans="12:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L17" s="2" t="s">
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="19"/>
+    </row>
+    <row r="12" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L12" s="12"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="13"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="22"/>
+    </row>
+    <row r="13" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L13" s="12"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="13"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="22"/>
+    </row>
+    <row r="14" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L14" s="12"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="13"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="22"/>
+    </row>
+    <row r="15" spans="12:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L15" s="14"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="16"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="25"/>
+    </row>
+    <row r="16" spans="12:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="17" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L17" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="4"/>
-      <c r="R17" s="2" t="s">
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="11"/>
+      <c r="R17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="4"/>
-    </row>
-    <row r="18" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L18" s="5"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="7"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="7"/>
-    </row>
-    <row r="19" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L19" s="5"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="7"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="7"/>
-    </row>
-    <row r="20" spans="12:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L20" s="8"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="10"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="10"/>
-    </row>
-    <row r="21" spans="12:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L22" s="2" t="s">
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="11"/>
+    </row>
+    <row r="18" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L18" s="12"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="13"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="13"/>
+    </row>
+    <row r="19" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L19" s="12"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="13"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="13"/>
+    </row>
+    <row r="20" spans="12:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L20" s="14"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="16"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="16"/>
+    </row>
+    <row r="21" spans="12:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="22" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L22" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="4"/>
-      <c r="R22" s="11" t="s">
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="11"/>
+      <c r="R22" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="S22" s="12"/>
-      <c r="T22" s="12"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="13"/>
-    </row>
-    <row r="23" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L23" s="5"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="7"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="16"/>
-    </row>
-    <row r="24" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L24" s="5"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="7"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="16"/>
-    </row>
-    <row r="25" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L25" s="5"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="7"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
-      <c r="U25" s="15"/>
-      <c r="V25" s="16"/>
-    </row>
-    <row r="26" spans="12:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L26" s="8"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="10"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="18"/>
-      <c r="U26" s="18"/>
-      <c r="V26" s="19"/>
-    </row>
-    <row r="29" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L29" s="20" t="s">
+      <c r="S22" s="18"/>
+      <c r="T22" s="18"/>
+      <c r="U22" s="18"/>
+      <c r="V22" s="19"/>
+    </row>
+    <row r="23" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L23" s="12"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="13"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="V23" s="22"/>
+    </row>
+    <row r="24" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L24" s="12"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="13"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="22"/>
+    </row>
+    <row r="25" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L25" s="12"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="13"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="22"/>
+    </row>
+    <row r="26" spans="12:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L26" s="14"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="16"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
+      <c r="U26" s="24"/>
+      <c r="V26" s="25"/>
+    </row>
+    <row r="29" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="M29" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-    </row>
-    <row r="30" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L30" s="21" t="s">
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+    </row>
+    <row r="30" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="M30" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-    </row>
-    <row r="31" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L31" s="21" t="s">
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+    </row>
+    <row r="31" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="M31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-    </row>
-    <row r="32" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L32" s="21" t="s">
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+    </row>
+    <row r="32" spans="12:22" x14ac:dyDescent="0.45">
+      <c r="L32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="M32" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-    </row>
-    <row r="33" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L33" s="21" t="s">
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+    </row>
+    <row r="33" spans="12:16" x14ac:dyDescent="0.45">
+      <c r="L33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="M33" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="M30:P30"/>
-    <mergeCell ref="M31:P31"/>
-    <mergeCell ref="M32:P32"/>
-    <mergeCell ref="M33:P33"/>
-    <mergeCell ref="M29:P29"/>
     <mergeCell ref="L22:P26"/>
     <mergeCell ref="L17:P20"/>
     <mergeCell ref="L11:P15"/>
@@ -1430,6 +1433,11 @@
     <mergeCell ref="R11:V15"/>
     <mergeCell ref="R17:V20"/>
     <mergeCell ref="R22:V26"/>
+    <mergeCell ref="M30:P30"/>
+    <mergeCell ref="M31:P31"/>
+    <mergeCell ref="M32:P32"/>
+    <mergeCell ref="M33:P33"/>
+    <mergeCell ref="M29:P29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1441,130 +1449,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D14AB2-F52E-4DD9-A15D-BE8C96E0B815}">
   <dimension ref="B2:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:2" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="2:2" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+    <row r="4" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="24"/>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B8" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
+    <row r="12" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="24"/>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B16" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
+    <row r="19" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="B19" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="24"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="24" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="24" t="s">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B23" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="B26" s="23" t="s">
+    <row r="26" spans="2:2" ht="17.649999999999999" x14ac:dyDescent="0.45">
+      <c r="B26" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="24"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="24" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B28" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="24" t="s">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B29" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="25" t="s">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B30" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>40</v>
       </c>
@@ -1578,19 +1586,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125B7970-CEBB-4BD7-B026-8887C851E1C4}">
   <dimension ref="B2:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.59765625" customWidth="1"/>
+    <col min="4" max="4" width="15.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>41</v>
       </c>
@@ -1598,7 +1606,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>43</v>
       </c>
@@ -1606,7 +1614,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>45</v>
       </c>
@@ -1614,17 +1622,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>49</v>
       </c>
@@ -1632,7 +1640,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>50</v>
       </c>
@@ -1640,7 +1648,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
       <c r="D15" t="s">
         <v>53</v>
       </c>
@@ -1648,17 +1659,20 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
       <c r="D17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="26">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D19" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F20" t="s">
         <v>56</v>
       </c>

</xml_diff>